<commit_message>
Update Module Don Thuoc
</commit_message>
<xml_diff>
--- a/public/thongke/ExportBenhNhanTrongNgay.xlsx
+++ b/public/thongke/ExportBenhNhanTrongNgay.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>Mã đơn thuốc</t>
   </si>
@@ -44,55 +44,112 @@
     <t>Số ngày dùng thuốc</t>
   </si>
   <si>
-    <t>TT2209270001</t>
-  </si>
-  <si>
-    <t>BN2209270001</t>
-  </si>
-  <si>
-    <t>Trần Văn Anh</t>
+    <t>TT2210110001</t>
+  </si>
+  <si>
+    <t>BN2210110001</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn A</t>
   </si>
   <si>
     <t>Nam</t>
   </si>
   <si>
-    <t>01-01-2022</t>
-  </si>
-  <si>
-    <t>27-09-2022 00:28:46</t>
-  </si>
-  <si>
-    <t>Covid</t>
-  </si>
-  <si>
-    <t>Đơn Lưu Cố Định</t>
+    <t>01-01-2000</t>
+  </si>
+  <si>
+    <t>11-10-2022 11:08:47</t>
+  </si>
+  <si>
+    <t>Viêm họng</t>
+  </si>
+  <si>
+    <t>Đơn lưu cố định</t>
   </si>
   <si>
     <t>15 ngày</t>
   </si>
   <si>
-    <t>TT2209270002</t>
-  </si>
-  <si>
-    <t>BN2209270002</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Tí</t>
-  </si>
-  <si>
-    <t>27-09-1999</t>
-  </si>
-  <si>
-    <t>27-09-2022 11:47:19</t>
-  </si>
-  <si>
-    <t>đâsdasd</t>
-  </si>
-  <si>
-    <t>Đơn In Cho Bệnh Nhân</t>
-  </si>
-  <si>
-    <t>20 ngày</t>
+    <t>TT2210110002</t>
+  </si>
+  <si>
+    <t>BN2210110002</t>
+  </si>
+  <si>
+    <t>11-10-2022 11:15:00</t>
+  </si>
+  <si>
+    <t>Đơn in cho nhà thuốc</t>
+  </si>
+  <si>
+    <t>TT2210110003</t>
+  </si>
+  <si>
+    <t>BN2210110003</t>
+  </si>
+  <si>
+    <t>11-10-2022 11:28:30</t>
+  </si>
+  <si>
+    <t>10 ngày</t>
+  </si>
+  <si>
+    <t>TT2210110004</t>
+  </si>
+  <si>
+    <t>BN2210110004</t>
+  </si>
+  <si>
+    <t>Lê Thanh Phúc</t>
+  </si>
+  <si>
+    <t>09-09-1999</t>
+  </si>
+  <si>
+    <t>11-10-2022 11:31:17</t>
+  </si>
+  <si>
+    <t>TT2210110005</t>
+  </si>
+  <si>
+    <t>BN2210110005</t>
+  </si>
+  <si>
+    <t>11-10-2022 11:40:42</t>
+  </si>
+  <si>
+    <t>30 ngày</t>
+  </si>
+  <si>
+    <t>TT2210110006</t>
+  </si>
+  <si>
+    <t>BN2210110006</t>
+  </si>
+  <si>
+    <t>11-10-2022 11:41:34</t>
+  </si>
+  <si>
+    <t>TT2210110007</t>
+  </si>
+  <si>
+    <t>BN2210110007</t>
+  </si>
+  <si>
+    <t>11-10-2022 12:05:59</t>
+  </si>
+  <si>
+    <t>TT2210110008</t>
+  </si>
+  <si>
+    <t>BN2210110008</t>
+  </si>
+  <si>
+    <t>01-01-1999</t>
+  </si>
+  <si>
+    <t>11-10-2022 14:07:53</t>
   </si>
 </sst>
 </file>
@@ -428,7 +485,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,24 +582,198 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" t="s">
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>